<commit_message>
conexión a sql Lima y Panamá
</commit_message>
<xml_diff>
--- a/check_PLs_ingreso.xlsx
+++ b/check_PLs_ingreso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inteligo\doc\tareas-data\rentabilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B98ADD7-214D-4B11-BE23-2DA5ABAB78BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B545CA-39FC-4E27-AF80-AE82E08F1DA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="205">
   <si>
     <t>DIFICULTAD DE ACCESO</t>
   </si>
@@ -616,6 +616,51 @@
   </si>
   <si>
     <t>Preguntar información a TI sobre los portafolios 14690-4 Income basket y 14690-15 estef(inteligo short time ...) se debe de realizar:  Sumar el número de cuotas que tiene el cliente al cerrar el mes. Ojo los martes se realizan rescates. Cuántas cuotas tenía el cliente al momento que se cobró.</t>
+  </si>
+  <si>
+    <t>comisión de custodia que cobra le banco. El cobro es semenstral.</t>
+  </si>
+  <si>
+    <t>cobro por cada transacción que realiza el cliente de pependiendo al grupo que pertenece.</t>
+  </si>
+  <si>
+    <t>Ingreso por comisión que cobra inteligo por colocación de fondos de terceros.</t>
+  </si>
+  <si>
+    <t>comisión por suscripción por fondo de tercero</t>
+  </si>
+  <si>
+    <t>comisión a los portafolios DIMA</t>
+  </si>
+  <si>
+    <t>son las notas a mercado.</t>
+  </si>
+  <si>
+    <t>comisión de salida de un producto estructurado, mínimo de 150</t>
+  </si>
+  <si>
+    <t>Revisar con Nelly - contabilidad</t>
+  </si>
+  <si>
+    <t>Revisar con Sr. Rogelio.</t>
+  </si>
+  <si>
+    <t>Es una comisión de manejo, es un manejo de productos privados. Datacapture. Pedir la lista de DC y porder filtrarlos por las referecnias de mag. Fee.</t>
+  </si>
+  <si>
+    <t>Averiguar</t>
+  </si>
+  <si>
+    <t>manejo igual al 52554</t>
+  </si>
+  <si>
+    <t>Revisar con el Sr. Rogelio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son registros manuales de Datacapture. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gasto por transacciones, el cobro que hace el custodio cada vez que se coloca una orden de compra o venda de fondos de tercero. El monto es asumido por le banco. </t>
   </si>
 </sst>
 </file>
@@ -721,7 +766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -761,6 +806,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
@@ -916,7 +967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1110,899 +1161,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2246,6 +1411,894 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2873,6 +2926,7 @@
           <cell r="O17">
             <v>0</v>
           </cell>
+          <cell r="P17"/>
           <cell r="Q17">
             <v>27585</v>
           </cell>
@@ -3199,6 +3253,7 @@
           <cell r="O24">
             <v>0</v>
           </cell>
+          <cell r="P24"/>
           <cell r="Q24">
             <v>0</v>
           </cell>
@@ -4056,64 +4111,64 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CE2F5A2-31AE-47D8-B3EC-7624EC051AA5}" name="Tabla2" displayName="Tabla2" ref="A2:J4" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CE2F5A2-31AE-47D8-B3EC-7624EC051AA5}" name="Tabla2" displayName="Tabla2" ref="A2:J4" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="A2:J4" xr:uid="{2499BF76-962C-41C0-AD74-80A51C5F99D3}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B5F99A9F-1039-4B19-BBCB-A41778D6EEBB}" name="PL" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{6832D3C1-7139-44FC-8174-8E4FFB48DCF7}" name="Descripción" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{112BB5CB-B54F-4D07-BF43-ECB8A7B21D09}" name="Disponible" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{B5F99A9F-1039-4B19-BBCB-A41778D6EEBB}" name="PL" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{6832D3C1-7139-44FC-8174-8E4FFB48DCF7}" name="Descripción" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{112BB5CB-B54F-4D07-BF43-ECB8A7B21D09}" name="Disponible" dataDxfId="41">
       <calculatedColumnFormula>VLOOKUP(Tabla2[[#This Row],[PL]],Tabla4[[PL]:[DISPONIBLE]],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C94BBD4B-6419-4AD1-9DD7-68C16579CBDA}" name="ID" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{C94BBD4B-6419-4AD1-9DD7-68C16579CBDA}" name="ID" dataDxfId="40">
       <calculatedColumnFormula>VLOOKUP(Tabla2[[#This Row],[PL]],PLs!C2:G25,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{EFE4E4A4-2A4A-4E7D-89FC-D44CB1B76294}" name="INDEX" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{C1846586-1ADA-427A-9F88-B83A98CFBC92}" name="MONTO ACUMULADO 2020" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{E1324BCA-3A50-4D0B-95D2-4DB7493854E6}" name="Contacto" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{1A8073B9-CC5A-41BE-8639-FA932788494F}" name="Cliente Cero" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{B06BD1E3-161E-472B-87C3-DDEA609ABAEB}" name="Monto Cli. Cero acumulado 2020" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{F356BAC1-6AB0-43FE-99B0-0ECCED9B633A}" name="Comentarios" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{EFE4E4A4-2A4A-4E7D-89FC-D44CB1B76294}" name="INDEX" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{C1846586-1ADA-427A-9F88-B83A98CFBC92}" name="MONTO ACUMULADO 2020" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{E1324BCA-3A50-4D0B-95D2-4DB7493854E6}" name="Contacto" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{1A8073B9-CC5A-41BE-8639-FA932788494F}" name="Cliente Cero" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{B06BD1E3-161E-472B-87C3-DDEA609ABAEB}" name="Monto Cli. Cero acumulado 2020" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{F356BAC1-6AB0-43FE-99B0-0ECCED9B633A}" name="Comentarios" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A566F06-45B6-42C1-9228-4DA8CEEA7E0E}" name="Tabla3" displayName="Tabla3" ref="A7:J32" totalsRowShown="0" headerRowDxfId="1" dataDxfId="28" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A566F06-45B6-42C1-9228-4DA8CEEA7E0E}" name="Tabla3" displayName="Tabla3" ref="A7:J32" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A7:J32" xr:uid="{24CF76C4-8FFE-435C-B9B3-D4A2C696A79D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:F32">
     <sortCondition descending="1" ref="F7:F32"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8B866B3F-E687-4F92-8961-256B372BA861}" name="PL" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{2613746C-E274-4591-B723-C786C7224306}" name="Descripción" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{08F8FB3D-FF3D-4665-B864-5865B0E7A110}" name="Disponible" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{8B866B3F-E687-4F92-8961-256B372BA861}" name="PL" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{2613746C-E274-4591-B723-C786C7224306}" name="Descripción" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{08F8FB3D-FF3D-4665-B864-5865B0E7A110}" name="Disponible" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP(Tabla3[[#This Row],[PL]],Tabla4[[PL]:[DISPONIBLE]],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6E0EA72-3A9C-4C46-B614-21967A0C9DE4}" name="ID" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{C6E0EA72-3A9C-4C46-B614-21967A0C9DE4}" name="ID" dataDxfId="25">
       <calculatedColumnFormula>VLOOKUP(Tabla3[[#This Row],[Descripción]],PLs!C2:F25,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{43F1CEAA-4CDF-4357-86ED-B27538F140AD}" name="INDEX" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{28A8DC59-3634-4397-B5A0-EA514DFAB7DA}" name="MONTO ACUMULADO 2020" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{43F1CEAA-4CDF-4357-86ED-B27538F140AD}" name="INDEX" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{28A8DC59-3634-4397-B5A0-EA514DFAB7DA}" name="MONTO ACUMULADO 2020" dataDxfId="23">
       <calculatedColumnFormula>VLOOKUP(Tabla3[[#This Row],[PL]],'[1]Fee Income'!$C$5:$Q$42,15,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E63CFCF9-27A0-4F79-BCFF-21D78E6B7DBE}" name="Contacto" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{5F9BEFC4-834F-4131-B9D0-5C5B4517C37F}" name="Cliente Cero" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{EF2E2DFA-A3D0-4793-97CA-BF6BE3C6399E}" name="Monto Cli. Cero acumulado 2020" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{A07F1565-8E21-44EA-B99D-1D8BA0FB2D7D}" name="Comentarios" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{E63CFCF9-27A0-4F79-BCFF-21D78E6B7DBE}" name="Contacto" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{5F9BEFC4-834F-4131-B9D0-5C5B4517C37F}" name="Cliente Cero" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{EF2E2DFA-A3D0-4793-97CA-BF6BE3C6399E}" name="Monto Cli. Cero acumulado 2020" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{A07F1565-8E21-44EA-B99D-1D8BA0FB2D7D}" name="Comentarios" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{44C9B693-3391-4861-8E8F-6AA7D2996C09}" name="Tabla26" displayName="Tabla26" ref="A2:J5" totalsRowShown="0" headerRowDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{44C9B693-3391-4861-8E8F-6AA7D2996C09}" name="Tabla26" displayName="Tabla26" ref="A2:J5" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A2:J5" xr:uid="{BD7EE68D-D9EE-4AD3-AB1C-2F9521548A30}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{10DAB0C4-4AFD-49A0-B3E5-749A6366A304}" name="PL" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{0CF8CA3C-6D20-4A3F-9961-FC92A1981E9D}" name="Descripción" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{408D760F-B776-4EC5-8B7A-A5F493245FDC}" name="Disponible" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{57432ECE-F737-4792-ACE7-A4FB56A03A7C}" name="ID" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{10DAB0C4-4AFD-49A0-B3E5-749A6366A304}" name="PL" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{0CF8CA3C-6D20-4A3F-9961-FC92A1981E9D}" name="Descripción" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{408D760F-B776-4EC5-8B7A-A5F493245FDC}" name="Disponible" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{57432ECE-F737-4792-ACE7-A4FB56A03A7C}" name="ID" dataDxfId="13"/>
     <tableColumn id="5" xr3:uid="{3C85AB5F-FBFE-4A68-B117-CAA9BDB4EF35}" name="INDEX"/>
     <tableColumn id="6" xr3:uid="{4E2AABC0-112D-408A-9FE9-31C7CA71FDF7}" name="MONTO ACUMULADO 2020"/>
     <tableColumn id="8" xr3:uid="{79BA7D35-6F10-431F-B7A1-4CF242A89DC3}" name="Contacto"/>
@@ -4147,22 +4202,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2090F493-EEA4-4C5A-8466-F9DD7FB3F963}" name="Tabla1" displayName="Tabla1" ref="A1:J45" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2090F493-EEA4-4C5A-8466-F9DD7FB3F963}" name="Tabla1" displayName="Tabla1" ref="A1:J45" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:J45" xr:uid="{72F5D041-3A51-47FE-8FF7-F2370AC54E5C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J45">
     <sortCondition ref="B1"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7D1CE239-8582-4EAE-B7D2-06FC3B060ED8}" name="Type" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{ACF15C81-9954-4215-9E73-021657EF82E6}" name="INDEX" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{35B6220B-80E4-4AA2-9A4E-3B0B94C1A477}" name="ID" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{31117B7A-7CD2-4557-AA88-5E3082E20AC0}" name="PL" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{DBDB2ED9-BC75-487A-8863-C45AEB4A8970}" name="Description" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{5621AFD6-B6AC-4969-BB32-FF503EDB1DE5}" name="TENR EN CUENTA" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{C49F3770-787B-4DE9-BEC1-9D73228BCB65}" name="DISPONIBLE" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{1FC93063-339C-4347-9DC4-2D634DA7250D}" name="ACCESO POR" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{9BEEAFC9-A1EE-48B6-A5B8-16998FBDEB8E}" name="CLIENTE CERO" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{9B2100A9-548F-42E2-AD5E-665A22348871}" name="Comentario" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{7D1CE239-8582-4EAE-B7D2-06FC3B060ED8}" name="Type" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{ACF15C81-9954-4215-9E73-021657EF82E6}" name="INDEX" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{35B6220B-80E4-4AA2-9A4E-3B0B94C1A477}" name="ID" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{31117B7A-7CD2-4557-AA88-5E3082E20AC0}" name="PL" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{DBDB2ED9-BC75-487A-8863-C45AEB4A8970}" name="Description" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{5621AFD6-B6AC-4969-BB32-FF503EDB1DE5}" name="TENR EN CUENTA" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{C49F3770-787B-4DE9-BEC1-9D73228BCB65}" name="DISPONIBLE" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{1FC93063-339C-4347-9DC4-2D634DA7250D}" name="ACCESO POR" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{9BEEAFC9-A1EE-48B6-A5B8-16998FBDEB8E}" name="CLIENTE CERO" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{9B2100A9-548F-42E2-AD5E-665A22348871}" name="Comentario" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4433,22 +4488,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA5A9AC-897C-4C4B-8E15-C77654157D01}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="4.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
     <col min="9" max="9" width="32.85546875" customWidth="1"/>
-    <col min="10" max="10" width="115.28515625" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
@@ -4643,7 +4698,9 @@
       <c r="I9" s="89">
         <v>-330755.71000000002</v>
       </c>
-      <c r="J9" s="62"/>
+      <c r="J9" s="62" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="87">
@@ -4673,7 +4730,9 @@
       <c r="I10" s="89">
         <v>93953.87</v>
       </c>
-      <c r="J10" s="62"/>
+      <c r="J10" s="62" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="79">
@@ -4703,7 +4762,9 @@
       <c r="I11" s="89">
         <v>178042.56</v>
       </c>
-      <c r="J11" s="62"/>
+      <c r="J11" s="62" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="79">
@@ -4733,7 +4794,9 @@
       <c r="I12" s="89">
         <v>70074.86</v>
       </c>
-      <c r="J12" s="62"/>
+      <c r="J12" s="62" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="79">
@@ -4763,7 +4826,9 @@
       <c r="I13" s="89">
         <v>3438.04</v>
       </c>
-      <c r="J13" s="62"/>
+      <c r="J13" s="62" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="87">
@@ -4825,13 +4890,15 @@
         <v>180</v>
       </c>
       <c r="I15" s="89"/>
-      <c r="J15" s="62"/>
+      <c r="J15" s="62" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="87">
+      <c r="A16" s="95">
         <v>53505</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="96" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="62" t="str">
@@ -4915,7 +4982,9 @@
       <c r="I18" s="89">
         <v>257841</v>
       </c>
-      <c r="J18" s="62"/>
+      <c r="J18" s="62" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="79">
@@ -5001,7 +5070,9 @@
         <v>180</v>
       </c>
       <c r="I21" s="89"/>
-      <c r="J21" s="62"/>
+      <c r="J21" s="62" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="79">
@@ -5029,7 +5100,9 @@
         <v>180</v>
       </c>
       <c r="I22" s="89"/>
-      <c r="J22" s="62"/>
+      <c r="J22" s="62" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="87">
@@ -5059,7 +5132,9 @@
       <c r="I23" s="89">
         <v>338.2</v>
       </c>
-      <c r="J23" s="62"/>
+      <c r="J23" s="62" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="79">
@@ -5087,7 +5162,9 @@
         <v>180</v>
       </c>
       <c r="I24" s="89"/>
-      <c r="J24" s="62"/>
+      <c r="J24" s="62" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="79">
@@ -5145,7 +5222,9 @@
         <v>180</v>
       </c>
       <c r="I26" s="88"/>
-      <c r="J26" s="62"/>
+      <c r="J26" s="62" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="87">
@@ -5173,7 +5252,9 @@
         <v>180</v>
       </c>
       <c r="I27" s="88"/>
-      <c r="J27" s="62"/>
+      <c r="J27" s="62" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="87">
@@ -5201,7 +5282,9 @@
         <v>180</v>
       </c>
       <c r="I28" s="88"/>
-      <c r="J28" s="62"/>
+      <c r="J28" s="62" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="79">
@@ -5257,7 +5340,9 @@
         <v>180</v>
       </c>
       <c r="I30" s="88"/>
-      <c r="J30" s="62"/>
+      <c r="J30" s="62" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="87">
@@ -5285,7 +5370,9 @@
         <v>180</v>
       </c>
       <c r="I31" s="88"/>
-      <c r="J31" s="62"/>
+      <c r="J31" s="62" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="90">
@@ -5331,7 +5418,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>